<commit_message>
Update test sprint 1,2,3
</commit_message>
<xml_diff>
--- a/Document/8.1.ProjectTestCaseSprint1.xlsx
+++ b/Document/8.1.ProjectTestCaseSprint1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A67617-9553-4526-86AF-9FEE8A706972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC122093-E40A-45FC-86FC-FE7E8AA0F74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="896" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trường hợp kiểm thử" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="529">
   <si>
     <t>TEST CASE SYSTEM SPRINT 1</t>
   </si>
@@ -1842,6 +1842,12 @@
   </si>
   <si>
     <t>Giao diện [Sản phẩm tương tự] không hiển thị và chưa được xử lý</t>
+  </si>
+  <si>
+    <t>Button [Đã hiểu] không biến mất, không thể quay lại màn hình</t>
+  </si>
+  <si>
+    <t>Không thể thấy giao diện "Xem thông tin đơn hàng"</t>
   </si>
 </sst>
 </file>
@@ -2464,7 +2470,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2843,18 +2849,42 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2870,30 +2900,6 @@
     <xf numFmtId="15" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2912,29 +2918,44 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4021,10 +4042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -4180,12 +4201,6 @@
       </c>
       <c r="E10" s="131" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="D11" s="8">
-        <f>SUM(D5:D10)</f>
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4218,24 +4233,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="24.6">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="161"/>
-      <c r="P1" s="161"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
+      <c r="P1" s="154"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="13.2">
       <c r="A2" s="2"/>
@@ -4259,22 +4274,22 @@
       <c r="A3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="162" t="s">
+      <c r="B3" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="162"/>
+      <c r="C3" s="155"/>
       <c r="D3" s="59"/>
-      <c r="E3" s="149" t="s">
+      <c r="E3" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="155" t="s">
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="157"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="150"/>
       <c r="L3" s="60"/>
       <c r="M3" s="60"/>
       <c r="N3" s="60"/>
@@ -4283,20 +4298,20 @@
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" ht="16.8">
       <c r="A4" s="58"/>
-      <c r="B4" s="148"/>
-      <c r="C4" s="148"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
       <c r="D4" s="61"/>
-      <c r="E4" s="149" t="s">
+      <c r="E4" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="149"/>
-      <c r="G4" s="149"/>
-      <c r="H4" s="158" t="s">
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="160"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="153"/>
       <c r="L4" s="61"/>
       <c r="M4" s="60"/>
       <c r="N4" s="60"/>
@@ -4305,20 +4320,20 @@
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" ht="16.8">
       <c r="A5" s="58"/>
-      <c r="B5" s="148"/>
-      <c r="C5" s="148"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="61"/>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="152">
+      <c r="F5" s="147"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="160">
         <v>44114</v>
       </c>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
-      <c r="K5" s="154"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="162"/>
       <c r="L5" s="61"/>
       <c r="M5" s="60"/>
       <c r="N5" s="60"/>
@@ -4329,18 +4344,18 @@
       <c r="A6" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="150" t="s">
+      <c r="B6" s="158" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150"/>
-      <c r="F6" s="150"/>
-      <c r="G6" s="150"/>
-      <c r="H6" s="150"/>
-      <c r="I6" s="150"/>
-      <c r="J6" s="150"/>
-      <c r="K6" s="150"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
+      <c r="F6" s="158"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="158"/>
+      <c r="K6" s="158"/>
       <c r="L6" s="63"/>
       <c r="M6" s="64"/>
       <c r="N6" s="64"/>
@@ -4350,52 +4365,52 @@
     <row r="7" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
       <c r="A7" s="65"/>
       <c r="B7" s="66"/>
-      <c r="C7" s="151" t="s">
+      <c r="C7" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="151"/>
-      <c r="E7" s="151" t="s">
+      <c r="D7" s="159"/>
+      <c r="E7" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="151"/>
-      <c r="G7" s="151" t="s">
+      <c r="F7" s="159"/>
+      <c r="G7" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="151"/>
-      <c r="I7" s="151" t="s">
+      <c r="H7" s="159"/>
+      <c r="I7" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="151"/>
-      <c r="K7" s="151" t="s">
+      <c r="J7" s="159"/>
+      <c r="K7" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="151"/>
-      <c r="M7" s="146" t="s">
+      <c r="L7" s="159"/>
+      <c r="M7" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="146"/>
-      <c r="O7" s="147" t="s">
+      <c r="N7" s="156"/>
+      <c r="O7" s="157" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="147"/>
+      <c r="P7" s="157"/>
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" ht="16.8">
       <c r="A8" s="67"/>
       <c r="B8" s="68"/>
-      <c r="C8" s="151"/>
-      <c r="D8" s="151"/>
-      <c r="E8" s="151"/>
-      <c r="F8" s="151"/>
-      <c r="G8" s="151"/>
-      <c r="H8" s="151"/>
-      <c r="I8" s="151"/>
-      <c r="J8" s="151"/>
-      <c r="K8" s="151"/>
-      <c r="L8" s="151"/>
-      <c r="M8" s="146"/>
-      <c r="N8" s="146"/>
-      <c r="O8" s="147"/>
-      <c r="P8" s="147"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
+      <c r="E8" s="159"/>
+      <c r="F8" s="159"/>
+      <c r="G8" s="159"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="159"/>
+      <c r="J8" s="159"/>
+      <c r="K8" s="159"/>
+      <c r="L8" s="159"/>
+      <c r="M8" s="156"/>
+      <c r="N8" s="156"/>
+      <c r="O8" s="157"/>
+      <c r="P8" s="157"/>
     </row>
     <row r="9" spans="1:16" s="5" customFormat="1" ht="22.5" customHeight="1">
       <c r="A9" s="69" t="s">
@@ -5116,13 +5131,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
     <mergeCell ref="M7:N8"/>
     <mergeCell ref="O7:P8"/>
     <mergeCell ref="B5:C5"/>
@@ -5134,6 +5142,13 @@
     <mergeCell ref="I7:J8"/>
     <mergeCell ref="K7:L8"/>
     <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -5144,8 +5159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="G14" zoomScale="72" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:K30"/>
+    <sheetView zoomScale="46" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -5222,10 +5237,10 @@
         <v>46</v>
       </c>
       <c r="B4" s="46">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C4" s="46">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="43">
         <f>COUNTIF(G11:G25,"Untested")</f>
@@ -5235,7 +5250,9 @@
         <f>COUNTIF(G11:G25,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F4" s="43"/>
+      <c r="F4" s="43">
+        <v>19</v>
+      </c>
       <c r="G4" s="29"/>
       <c r="H4" s="30"/>
       <c r="J4" s="29"/>
@@ -5244,7 +5261,9 @@
       <c r="A5" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="46"/>
+      <c r="B5" s="46">
+        <v>19</v>
+      </c>
       <c r="C5" s="46">
         <v>0</v>
       </c>
@@ -5256,7 +5275,9 @@
         <f>COUNTIF(J11:J25,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="43"/>
+      <c r="F5" s="43">
+        <v>19</v>
+      </c>
       <c r="G5" s="29"/>
       <c r="H5" s="30"/>
       <c r="J5" s="29"/>
@@ -5380,22 +5401,22 @@
       <c r="F11" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H11" s="54">
+      <c r="G11" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H11" s="178">
         <v>45781</v>
       </c>
-      <c r="I11" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K11" s="54">
+      <c r="I11" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K11" s="178">
         <v>45934</v>
       </c>
-      <c r="L11" s="55" t="s">
+      <c r="L11" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M11" s="81"/>
@@ -5415,22 +5436,22 @@
       <c r="F12" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="G12" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H12" s="54">
+      <c r="G12" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H12" s="178">
         <v>45781</v>
       </c>
-      <c r="I12" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K12" s="54">
+      <c r="I12" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K12" s="178">
         <v>45934</v>
       </c>
-      <c r="L12" s="55" t="s">
+      <c r="L12" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M12" s="81"/>
@@ -5450,22 +5471,22 @@
       <c r="F13" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H13" s="54">
+      <c r="G13" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H13" s="178">
         <v>45781</v>
       </c>
-      <c r="I13" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K13" s="54">
+      <c r="I13" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K13" s="178">
         <v>45934</v>
       </c>
-      <c r="L13" s="55" t="s">
+      <c r="L13" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M13" s="81"/>
@@ -5485,22 +5506,22 @@
       <c r="F14" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H14" s="54">
+      <c r="G14" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H14" s="178">
         <v>45781</v>
       </c>
-      <c r="I14" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K14" s="54">
+      <c r="I14" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K14" s="178">
         <v>45934</v>
       </c>
-      <c r="L14" s="55" t="s">
+      <c r="L14" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M14" s="81"/>
@@ -5520,22 +5541,22 @@
       <c r="F15" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H15" s="54">
+      <c r="G15" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H15" s="178">
         <v>45781</v>
       </c>
-      <c r="I15" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K15" s="54">
+      <c r="I15" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K15" s="178">
         <v>45934</v>
       </c>
-      <c r="L15" s="55" t="s">
+      <c r="L15" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M15" s="81"/>
@@ -5555,22 +5576,22 @@
       <c r="F16" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H16" s="54">
+      <c r="G16" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H16" s="178">
         <v>45781</v>
       </c>
-      <c r="I16" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K16" s="54">
+      <c r="I16" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K16" s="178">
         <v>45934</v>
       </c>
-      <c r="L16" s="55" t="s">
+      <c r="L16" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M16" s="81"/>
@@ -5590,22 +5611,22 @@
       <c r="F17" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H17" s="54">
+      <c r="G17" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H17" s="178">
         <v>45781</v>
       </c>
-      <c r="I17" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K17" s="54">
+      <c r="I17" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K17" s="178">
         <v>45934</v>
       </c>
-      <c r="L17" s="55" t="s">
+      <c r="L17" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M17" s="88"/>
@@ -5625,22 +5646,22 @@
       <c r="F18" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H18" s="54">
+      <c r="G18" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H18" s="178">
         <v>45781</v>
       </c>
-      <c r="I18" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K18" s="54">
+      <c r="I18" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K18" s="178">
         <v>45934</v>
       </c>
-      <c r="L18" s="55" t="s">
+      <c r="L18" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M18" s="88"/>
@@ -5660,22 +5681,22 @@
       <c r="F19" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H19" s="54">
+      <c r="G19" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H19" s="178">
         <v>45781</v>
       </c>
-      <c r="I19" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K19" s="54">
+      <c r="I19" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K19" s="178">
         <v>45934</v>
       </c>
-      <c r="L19" s="55" t="s">
+      <c r="L19" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M19" s="88"/>
@@ -5695,22 +5716,22 @@
       <c r="F20" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H20" s="54">
+      <c r="G20" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H20" s="178">
         <v>45781</v>
       </c>
-      <c r="I20" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K20" s="54">
+      <c r="I20" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K20" s="178">
         <v>45934</v>
       </c>
-      <c r="L20" s="55" t="s">
+      <c r="L20" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M20" s="88"/>
@@ -5749,22 +5770,22 @@
       <c r="F22" s="92" t="s">
         <v>486</v>
       </c>
-      <c r="G22" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H22" s="54">
+      <c r="G22" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H22" s="178">
         <v>45781</v>
       </c>
-      <c r="I22" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J22" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K22" s="54">
+      <c r="I22" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K22" s="178">
         <v>45934</v>
       </c>
-      <c r="L22" s="55" t="s">
+      <c r="L22" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M22" s="81"/>
@@ -5788,22 +5809,22 @@
       <c r="F23" s="124" t="s">
         <v>488</v>
       </c>
-      <c r="G23" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H23" s="54">
+      <c r="G23" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H23" s="178">
         <v>45781</v>
       </c>
-      <c r="I23" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J23" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K23" s="54">
+      <c r="I23" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K23" s="178">
         <v>45934</v>
       </c>
-      <c r="L23" s="55" t="s">
+      <c r="L23" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M23" s="81"/>
@@ -5827,22 +5848,22 @@
       <c r="F24" s="92" t="s">
         <v>490</v>
       </c>
-      <c r="G24" s="53" t="s">
+      <c r="G24" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="H24" s="54">
+      <c r="H24" s="178">
         <v>45781</v>
       </c>
-      <c r="I24" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" s="53" t="s">
+      <c r="I24" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="K24" s="54">
+      <c r="K24" s="178">
         <v>45934</v>
       </c>
-      <c r="L24" s="55" t="s">
+      <c r="L24" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M24" s="81"/>
@@ -5866,22 +5887,22 @@
       <c r="F25" s="124" t="s">
         <v>96</v>
       </c>
-      <c r="G25" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H25" s="54">
+      <c r="G25" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H25" s="178">
         <v>45781</v>
       </c>
-      <c r="I25" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K25" s="54">
+      <c r="I25" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K25" s="178">
         <v>45934</v>
       </c>
-      <c r="L25" s="55" t="s">
+      <c r="L25" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M25" s="81"/>
@@ -5905,22 +5926,22 @@
       <c r="F26" s="92" t="s">
         <v>491</v>
       </c>
-      <c r="G26" s="53" t="s">
+      <c r="G26" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="H26" s="54">
+      <c r="H26" s="178">
         <v>45781</v>
       </c>
-      <c r="I26" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J26" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K26" s="54">
+      <c r="I26" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K26" s="178">
         <v>45934</v>
       </c>
-      <c r="L26" s="55" t="s">
+      <c r="L26" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M26" s="81"/>
@@ -5944,22 +5965,22 @@
       <c r="F27" s="124" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H27" s="54">
+      <c r="G27" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H27" s="178">
         <v>45781</v>
       </c>
-      <c r="I27" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K27" s="54">
+      <c r="I27" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K27" s="178">
         <v>45934</v>
       </c>
-      <c r="L27" s="55" t="s">
+      <c r="L27" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M27" s="81"/>
@@ -5983,22 +6004,22 @@
       <c r="F28" s="92" t="s">
         <v>492</v>
       </c>
-      <c r="G28" s="53" t="s">
+      <c r="G28" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="H28" s="54">
+      <c r="H28" s="178">
         <v>45781</v>
       </c>
-      <c r="I28" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J28" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K28" s="54">
+      <c r="I28" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K28" s="178">
         <v>45934</v>
       </c>
-      <c r="L28" s="55" t="s">
+      <c r="L28" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M28" s="81"/>
@@ -6022,22 +6043,22 @@
       <c r="F29" s="92" t="s">
         <v>493</v>
       </c>
-      <c r="G29" s="53" t="s">
+      <c r="G29" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="H29" s="54">
+      <c r="H29" s="178">
         <v>45781</v>
       </c>
-      <c r="I29" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K29" s="54">
+      <c r="I29" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K29" s="178">
         <v>45934</v>
       </c>
-      <c r="L29" s="55" t="s">
+      <c r="L29" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M29" s="81"/>
@@ -6061,22 +6082,22 @@
       <c r="F30" s="92" t="s">
         <v>494</v>
       </c>
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="H30" s="54">
+      <c r="H30" s="178">
         <v>45781</v>
       </c>
-      <c r="I30" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K30" s="54">
+      <c r="I30" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K30" s="178">
         <v>45934</v>
       </c>
-      <c r="L30" s="55" t="s">
+      <c r="L30" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M30" s="81"/>
@@ -6128,8 +6149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="F15" zoomScale="54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:K46"/>
+    <sheetView zoomScale="54" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -6147,20 +6168,22 @@
     <col min="11" max="11" width="21.5546875" style="117" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" style="117" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="117" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="117"/>
+    <col min="14" max="14" width="9.109375" style="117"/>
+    <col min="15" max="15" width="11.5546875" style="117" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="117"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="97" customFormat="1" ht="24" customHeight="1">
       <c r="A1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
       <c r="G1" s="95"/>
       <c r="H1" s="96"/>
       <c r="J1" s="95"/>
@@ -6169,13 +6192,13 @@
       <c r="A2" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="174" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
       <c r="G2" s="95"/>
       <c r="H2" s="96"/>
       <c r="J2" s="95"/>
@@ -6206,10 +6229,10 @@
         <v>46</v>
       </c>
       <c r="B4" s="101">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C4" s="101">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D4" s="98">
         <f>COUNTIF(G11:G25,"Untested")</f>
@@ -6219,7 +6242,9 @@
         <f>COUNTIF(G11:G25,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F4" s="98"/>
+      <c r="F4" s="98">
+        <v>35</v>
+      </c>
       <c r="G4" s="95"/>
       <c r="H4" s="96"/>
       <c r="J4" s="95"/>
@@ -6228,7 +6253,9 @@
       <c r="A5" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="101">
+        <v>35</v>
+      </c>
       <c r="C5" s="101">
         <v>0</v>
       </c>
@@ -6240,7 +6267,9 @@
         <f>COUNTIF(J11:J25,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="98"/>
+      <c r="F5" s="98">
+        <v>35</v>
+      </c>
       <c r="G5" s="95"/>
       <c r="H5" s="96"/>
       <c r="J5" s="95"/>
@@ -6334,21 +6363,21 @@
       <c r="M9" s="171"/>
     </row>
     <row r="10" spans="1:13" s="97" customFormat="1">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="172" t="s">
         <v>170</v>
       </c>
-      <c r="B10" s="174"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="174"/>
-      <c r="E10" s="174"/>
-      <c r="F10" s="174"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="174"/>
-      <c r="K10" s="174"/>
-      <c r="L10" s="174"/>
-      <c r="M10" s="174"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="172"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="172"/>
+      <c r="L10" s="172"/>
+      <c r="M10" s="172"/>
     </row>
     <row r="11" spans="1:13" s="97" customFormat="1" ht="134.4">
       <c r="A11" s="108" t="s">
@@ -6365,22 +6394,22 @@
       <c r="F11" s="111" t="s">
         <v>203</v>
       </c>
-      <c r="G11" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H11" s="54">
+      <c r="G11" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H11" s="178">
         <v>45781</v>
       </c>
-      <c r="I11" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K11" s="54">
+      <c r="I11" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K11" s="178">
         <v>45934</v>
       </c>
-      <c r="L11" s="113" t="s">
+      <c r="L11" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M11" s="110"/>
@@ -6400,22 +6429,22 @@
       <c r="F12" s="111" t="s">
         <v>105</v>
       </c>
-      <c r="G12" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H12" s="54">
+      <c r="G12" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H12" s="178">
         <v>45781</v>
       </c>
-      <c r="I12" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K12" s="54">
+      <c r="I12" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K12" s="178">
         <v>45934</v>
       </c>
-      <c r="L12" s="113" t="s">
+      <c r="L12" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M12" s="110"/>
@@ -6435,22 +6464,22 @@
       <c r="F13" s="111" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H13" s="54">
+      <c r="G13" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H13" s="178">
         <v>45781</v>
       </c>
-      <c r="I13" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K13" s="54">
+      <c r="I13" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K13" s="178">
         <v>45934</v>
       </c>
-      <c r="L13" s="113" t="s">
+      <c r="L13" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M13" s="110"/>
@@ -6470,22 +6499,22 @@
       <c r="F14" s="132" t="s">
         <v>465</v>
       </c>
-      <c r="G14" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H14" s="54">
+      <c r="G14" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H14" s="178">
         <v>45781</v>
       </c>
-      <c r="I14" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K14" s="54">
+      <c r="I14" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K14" s="178">
         <v>45934</v>
       </c>
-      <c r="L14" s="113" t="s">
+      <c r="L14" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M14" s="110"/>
@@ -6505,22 +6534,22 @@
       <c r="F15" s="132" t="s">
         <v>467</v>
       </c>
-      <c r="G15" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H15" s="54">
+      <c r="G15" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H15" s="178">
         <v>45781</v>
       </c>
-      <c r="I15" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K15" s="54">
+      <c r="I15" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K15" s="178">
         <v>45934</v>
       </c>
-      <c r="L15" s="113" t="s">
+      <c r="L15" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M15" s="110"/>
@@ -6540,22 +6569,22 @@
       <c r="F16" s="132" t="s">
         <v>471</v>
       </c>
-      <c r="G16" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H16" s="54">
+      <c r="G16" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H16" s="178">
         <v>45781</v>
       </c>
-      <c r="I16" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K16" s="54">
+      <c r="I16" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K16" s="178">
         <v>45934</v>
       </c>
-      <c r="L16" s="113" t="s">
+      <c r="L16" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M16" s="110"/>
@@ -6575,22 +6604,22 @@
       <c r="F17" s="132" t="s">
         <v>469</v>
       </c>
-      <c r="G17" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H17" s="54">
+      <c r="G17" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H17" s="178">
         <v>45781</v>
       </c>
-      <c r="I17" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K17" s="54">
+      <c r="I17" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K17" s="178">
         <v>45934</v>
       </c>
-      <c r="L17" s="113" t="s">
+      <c r="L17" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M17" s="110"/>
@@ -6610,22 +6639,22 @@
       <c r="F18" s="132" t="s">
         <v>473</v>
       </c>
-      <c r="G18" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H18" s="54">
+      <c r="G18" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H18" s="178">
         <v>45781</v>
       </c>
-      <c r="I18" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K18" s="54">
+      <c r="I18" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K18" s="178">
         <v>45934</v>
       </c>
-      <c r="L18" s="113" t="s">
+      <c r="L18" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M18" s="110"/>
@@ -6645,22 +6674,22 @@
       <c r="F19" s="132" t="s">
         <v>475</v>
       </c>
-      <c r="G19" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H19" s="54">
+      <c r="G19" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H19" s="178">
         <v>45781</v>
       </c>
-      <c r="I19" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K19" s="54">
+      <c r="I19" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K19" s="178">
         <v>45934</v>
       </c>
-      <c r="L19" s="113" t="s">
+      <c r="L19" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M19" s="110"/>
@@ -6680,42 +6709,42 @@
       <c r="F20" s="132" t="s">
         <v>477</v>
       </c>
-      <c r="G20" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H20" s="54">
+      <c r="G20" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H20" s="178">
         <v>45781</v>
       </c>
-      <c r="I20" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K20" s="54">
+      <c r="I20" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K20" s="178">
         <v>45934</v>
       </c>
-      <c r="L20" s="113" t="s">
+      <c r="L20" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M20" s="110"/>
     </row>
     <row r="21" spans="1:13" s="97" customFormat="1">
-      <c r="A21" s="172" t="s">
+      <c r="A21" s="169" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="173"/>
-      <c r="C21" s="173"/>
-      <c r="D21" s="173"/>
-      <c r="E21" s="173"/>
-      <c r="F21" s="172"/>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172"/>
-      <c r="J21" s="172"/>
-      <c r="K21" s="172"/>
-      <c r="L21" s="172"/>
-      <c r="M21" s="172"/>
+      <c r="B21" s="170"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="170"/>
+      <c r="F21" s="169"/>
+      <c r="G21" s="169"/>
+      <c r="H21" s="169"/>
+      <c r="I21" s="169"/>
+      <c r="J21" s="169"/>
+      <c r="K21" s="169"/>
+      <c r="L21" s="169"/>
+      <c r="M21" s="169"/>
     </row>
     <row r="22" spans="1:13" s="97" customFormat="1" ht="67.2">
       <c r="A22" s="115" t="s">
@@ -6734,22 +6763,22 @@
       <c r="F22" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="G22" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H22" s="54">
+      <c r="G22" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H22" s="178">
         <v>45781</v>
       </c>
-      <c r="I22" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J22" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K22" s="54">
+      <c r="I22" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K22" s="178">
         <v>45934</v>
       </c>
-      <c r="L22" s="113" t="s">
+      <c r="L22" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M22" s="110"/>
@@ -6773,22 +6802,22 @@
       <c r="F23" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H23" s="54">
+      <c r="G23" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H23" s="178">
         <v>45781</v>
       </c>
-      <c r="I23" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J23" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K23" s="54">
+      <c r="I23" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K23" s="178">
         <v>45934</v>
       </c>
-      <c r="L23" s="113" t="s">
+      <c r="L23" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M23" s="110"/>
@@ -6812,22 +6841,22 @@
       <c r="F24" s="120" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H24" s="54">
+      <c r="G24" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H24" s="178">
         <v>45781</v>
       </c>
-      <c r="I24" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K24" s="54">
+      <c r="I24" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K24" s="178">
         <v>45934</v>
       </c>
-      <c r="L24" s="113" t="s">
+      <c r="L24" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M24" s="121"/>
@@ -6851,22 +6880,22 @@
       <c r="F25" s="120" t="s">
         <v>123</v>
       </c>
-      <c r="G25" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H25" s="54">
+      <c r="G25" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H25" s="178">
         <v>45781</v>
       </c>
-      <c r="I25" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K25" s="54">
+      <c r="I25" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K25" s="178">
         <v>45934</v>
       </c>
-      <c r="L25" s="113" t="s">
+      <c r="L25" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M25" s="120"/>
@@ -6890,22 +6919,22 @@
       <c r="F26" s="93" t="s">
         <v>126</v>
       </c>
-      <c r="G26" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H26" s="54">
+      <c r="G26" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H26" s="178">
         <v>45781</v>
       </c>
-      <c r="I26" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J26" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K26" s="54">
+      <c r="I26" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K26" s="178">
         <v>45934</v>
       </c>
-      <c r="L26" s="113" t="s">
+      <c r="L26" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M26" s="120"/>
@@ -6929,22 +6958,22 @@
       <c r="F27" s="120" t="s">
         <v>495</v>
       </c>
-      <c r="G27" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H27" s="54">
+      <c r="G27" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H27" s="178">
         <v>45781</v>
       </c>
-      <c r="I27" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K27" s="54">
+      <c r="I27" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K27" s="178">
         <v>45934</v>
       </c>
-      <c r="L27" s="113" t="s">
+      <c r="L27" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M27" s="120"/>
@@ -6968,22 +6997,22 @@
       <c r="F28" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H28" s="54">
+      <c r="G28" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H28" s="178">
         <v>45781</v>
       </c>
-      <c r="I28" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J28" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K28" s="54">
+      <c r="I28" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K28" s="178">
         <v>45934</v>
       </c>
-      <c r="L28" s="113" t="s">
+      <c r="L28" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M28" s="120"/>
@@ -7007,22 +7036,22 @@
       <c r="F29" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="G29" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H29" s="54">
+      <c r="G29" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H29" s="178">
         <v>45781</v>
       </c>
-      <c r="I29" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K29" s="54">
+      <c r="I29" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K29" s="178">
         <v>45934</v>
       </c>
-      <c r="L29" s="113" t="s">
+      <c r="L29" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M29" s="120"/>
@@ -7046,22 +7075,22 @@
       <c r="F30" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G30" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H30" s="54">
+      <c r="G30" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H30" s="178">
         <v>45781</v>
       </c>
-      <c r="I30" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K30" s="54">
+      <c r="I30" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K30" s="178">
         <v>45934</v>
       </c>
-      <c r="L30" s="113" t="s">
+      <c r="L30" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M30" s="120"/>
@@ -7085,22 +7114,22 @@
       <c r="F31" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G31" s="112" t="s">
+      <c r="G31" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H31" s="54">
+      <c r="H31" s="178">
         <v>45781</v>
       </c>
-      <c r="I31" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="112" t="s">
+      <c r="I31" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K31" s="54">
+      <c r="K31" s="178">
         <v>45934</v>
       </c>
-      <c r="L31" s="113" t="s">
+      <c r="L31" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M31" s="120"/>
@@ -7124,22 +7153,22 @@
       <c r="F32" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G32" s="112" t="s">
+      <c r="G32" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H32" s="54">
+      <c r="H32" s="178">
         <v>45781</v>
       </c>
-      <c r="I32" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J32" s="112" t="s">
+      <c r="I32" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K32" s="54">
+      <c r="K32" s="178">
         <v>45934</v>
       </c>
-      <c r="L32" s="113" t="s">
+      <c r="L32" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M32" s="120"/>
@@ -7163,22 +7192,22 @@
       <c r="F33" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G33" s="112" t="s">
+      <c r="G33" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H33" s="54">
+      <c r="H33" s="178">
         <v>45781</v>
       </c>
-      <c r="I33" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" s="112" t="s">
+      <c r="I33" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K33" s="54">
+      <c r="K33" s="178">
         <v>45934</v>
       </c>
-      <c r="L33" s="113" t="s">
+      <c r="L33" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M33" s="120"/>
@@ -7202,22 +7231,22 @@
       <c r="F34" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G34" s="112" t="s">
+      <c r="G34" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H34" s="54">
+      <c r="H34" s="178">
         <v>45781</v>
       </c>
-      <c r="I34" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J34" s="112" t="s">
+      <c r="I34" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K34" s="54">
+      <c r="K34" s="178">
         <v>45934</v>
       </c>
-      <c r="L34" s="113" t="s">
+      <c r="L34" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M34" s="120"/>
@@ -7241,22 +7270,22 @@
       <c r="F35" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G35" s="112" t="s">
+      <c r="G35" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H35" s="54">
+      <c r="H35" s="178">
         <v>45781</v>
       </c>
-      <c r="I35" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="112" t="s">
+      <c r="I35" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K35" s="54">
+      <c r="K35" s="178">
         <v>45934</v>
       </c>
-      <c r="L35" s="113" t="s">
+      <c r="L35" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M35" s="120"/>
@@ -7280,22 +7309,22 @@
       <c r="F36" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G36" s="112" t="s">
+      <c r="G36" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H36" s="54">
+      <c r="H36" s="178">
         <v>45781</v>
       </c>
-      <c r="I36" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" s="112" t="s">
+      <c r="I36" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K36" s="54">
+      <c r="K36" s="178">
         <v>45934</v>
       </c>
-      <c r="L36" s="113" t="s">
+      <c r="L36" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M36" s="120"/>
@@ -7319,22 +7348,22 @@
       <c r="F37" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G37" s="112" t="s">
+      <c r="G37" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H37" s="54">
+      <c r="H37" s="178">
         <v>45781</v>
       </c>
-      <c r="I37" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J37" s="112" t="s">
+      <c r="I37" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K37" s="54">
+      <c r="K37" s="178">
         <v>45934</v>
       </c>
-      <c r="L37" s="113" t="s">
+      <c r="L37" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M37" s="120"/>
@@ -7358,22 +7387,22 @@
       <c r="F38" s="120" t="s">
         <v>496</v>
       </c>
-      <c r="G38" s="112" t="s">
+      <c r="G38" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="H38" s="54">
+      <c r="H38" s="178">
         <v>45781</v>
       </c>
-      <c r="I38" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J38" s="112" t="s">
+      <c r="I38" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38" s="180" t="s">
         <v>489</v>
       </c>
-      <c r="K38" s="54">
+      <c r="K38" s="178">
         <v>45934</v>
       </c>
-      <c r="L38" s="113" t="s">
+      <c r="L38" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M38" s="120"/>
@@ -7397,22 +7426,22 @@
       <c r="F39" s="123" t="s">
         <v>497</v>
       </c>
-      <c r="G39" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H39" s="54">
+      <c r="G39" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H39" s="178">
         <v>45781</v>
       </c>
-      <c r="I39" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J39" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K39" s="54">
+      <c r="I39" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J39" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K39" s="178">
         <v>45934</v>
       </c>
-      <c r="L39" s="113" t="s">
+      <c r="L39" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M39" s="120"/>
@@ -7436,22 +7465,22 @@
       <c r="F40" s="120" t="s">
         <v>199</v>
       </c>
-      <c r="G40" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H40" s="54">
+      <c r="G40" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H40" s="178">
         <v>45781</v>
       </c>
-      <c r="I40" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J40" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K40" s="54">
+      <c r="I40" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J40" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K40" s="178">
         <v>45934</v>
       </c>
-      <c r="L40" s="113" t="s">
+      <c r="L40" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M40" s="120"/>
@@ -7475,22 +7504,22 @@
       <c r="F41" s="123" t="s">
         <v>420</v>
       </c>
-      <c r="G41" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H41" s="54">
+      <c r="G41" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H41" s="178">
         <v>45781</v>
       </c>
-      <c r="I41" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J41" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K41" s="54">
+      <c r="I41" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J41" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K41" s="178">
         <v>45934</v>
       </c>
-      <c r="L41" s="113" t="s">
+      <c r="L41" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M41" s="120"/>
@@ -7514,22 +7543,22 @@
       <c r="F42" s="123" t="s">
         <v>424</v>
       </c>
-      <c r="G42" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H42" s="54">
+      <c r="G42" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H42" s="178">
         <v>45781</v>
       </c>
-      <c r="I42" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J42" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K42" s="54">
+      <c r="I42" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J42" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K42" s="178">
         <v>45934</v>
       </c>
-      <c r="L42" s="113" t="s">
+      <c r="L42" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M42" s="120"/>
@@ -7553,22 +7582,22 @@
       <c r="F43" s="123" t="s">
         <v>498</v>
       </c>
-      <c r="G43" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H43" s="54">
+      <c r="G43" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H43" s="178">
         <v>45781</v>
       </c>
-      <c r="I43" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J43" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K43" s="54">
+      <c r="I43" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K43" s="178">
         <v>45934</v>
       </c>
-      <c r="L43" s="113" t="s">
+      <c r="L43" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M43" s="120"/>
@@ -7592,22 +7621,22 @@
       <c r="F44" s="123" t="s">
         <v>430</v>
       </c>
-      <c r="G44" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H44" s="54">
+      <c r="G44" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H44" s="178">
         <v>45781</v>
       </c>
-      <c r="I44" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J44" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K44" s="54">
+      <c r="I44" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J44" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K44" s="178">
         <v>45934</v>
       </c>
-      <c r="L44" s="113" t="s">
+      <c r="L44" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M44" s="120"/>
@@ -7631,22 +7660,22 @@
       <c r="F45" s="123" t="s">
         <v>500</v>
       </c>
-      <c r="G45" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H45" s="54">
+      <c r="G45" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H45" s="178">
         <v>45781</v>
       </c>
-      <c r="I45" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J45" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K45" s="54">
+      <c r="I45" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J45" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K45" s="178">
         <v>45934</v>
       </c>
-      <c r="L45" s="113" t="s">
+      <c r="L45" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M45" s="120"/>
@@ -7670,22 +7699,22 @@
       <c r="F46" s="123" t="s">
         <v>427</v>
       </c>
-      <c r="G46" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="H46" s="54">
+      <c r="G46" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="H46" s="178">
         <v>45781</v>
       </c>
-      <c r="I46" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="J46" s="112" t="s">
-        <v>487</v>
-      </c>
-      <c r="K46" s="54">
+      <c r="I46" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" s="180" t="s">
+        <v>487</v>
+      </c>
+      <c r="K46" s="178">
         <v>45934</v>
       </c>
-      <c r="L46" s="113" t="s">
+      <c r="L46" s="181" t="s">
         <v>63</v>
       </c>
       <c r="M46" s="120"/>
@@ -7760,13 +7789,6 @@
     <row r="63" spans="1:13" ht="103.8" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A21:M21"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A10:M10"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -7775,6 +7797,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A21:M21"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A10:M10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="J11:J20 G22:G46 G11:G20 J22:J46" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -7792,8 +7821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="G14" zoomScale="64" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScale="53" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -7818,13 +7847,13 @@
       <c r="A1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
       <c r="G1" s="95"/>
       <c r="H1" s="96"/>
       <c r="J1" s="95"/>
@@ -7833,13 +7862,13 @@
       <c r="A2" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="174" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
       <c r="G2" s="95"/>
       <c r="H2" s="96"/>
       <c r="J2" s="95"/>
@@ -7870,10 +7899,10 @@
         <v>46</v>
       </c>
       <c r="B4" s="101">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C4" s="101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="98">
         <f>COUNTIF(G11:G18,"Untested")</f>
@@ -7883,7 +7912,9 @@
         <f>COUNTIF(G11:G18,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F4" s="98"/>
+      <c r="F4" s="98">
+        <v>9</v>
+      </c>
       <c r="G4" s="95"/>
       <c r="H4" s="96"/>
       <c r="J4" s="95"/>
@@ -7892,7 +7923,9 @@
       <c r="A5" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="101">
+        <v>9</v>
+      </c>
       <c r="C5" s="101">
         <v>0</v>
       </c>
@@ -7904,7 +7937,9 @@
         <f>COUNTIF(J11:J18,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="98"/>
+      <c r="F5" s="98">
+        <v>9</v>
+      </c>
       <c r="G5" s="95"/>
       <c r="H5" s="96"/>
       <c r="J5" s="95"/>
@@ -8029,22 +8064,22 @@
       <c r="F11" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="G11" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H11" s="54">
+      <c r="G11" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H11" s="178">
         <v>45812</v>
       </c>
-      <c r="I11" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K11" s="54">
+      <c r="I11" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K11" s="178">
         <v>45965</v>
       </c>
-      <c r="L11" s="55" t="s">
+      <c r="L11" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M11" s="81"/>
@@ -8064,22 +8099,22 @@
       <c r="F12" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="G12" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H12" s="54">
+      <c r="G12" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H12" s="178">
         <v>45812</v>
       </c>
-      <c r="I12" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K12" s="54">
+      <c r="I12" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K12" s="178">
         <v>45965</v>
       </c>
-      <c r="L12" s="55" t="s">
+      <c r="L12" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M12" s="81"/>
@@ -8099,22 +8134,22 @@
       <c r="F13" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H13" s="54">
+      <c r="G13" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H13" s="178">
         <v>45812</v>
       </c>
-      <c r="I13" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K13" s="54">
+      <c r="I13" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K13" s="178">
         <v>45965</v>
       </c>
-      <c r="L13" s="55" t="s">
+      <c r="L13" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M13" s="81"/>
@@ -8153,22 +8188,22 @@
       <c r="F15" s="124" t="s">
         <v>210</v>
       </c>
-      <c r="G15" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H15" s="54">
+      <c r="G15" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H15" s="178">
         <v>45812</v>
       </c>
-      <c r="I15" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K15" s="54">
+      <c r="I15" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K15" s="178">
         <v>45965</v>
       </c>
-      <c r="L15" s="55" t="s">
+      <c r="L15" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M15" s="81"/>
@@ -8192,22 +8227,22 @@
       <c r="F16" s="92" t="s">
         <v>501</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H16" s="178">
         <v>45812</v>
       </c>
-      <c r="I16" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K16" s="54">
+      <c r="I16" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K16" s="178">
         <v>45965</v>
       </c>
-      <c r="L16" s="55" t="s">
+      <c r="L16" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M16" s="81"/>
@@ -8231,22 +8266,22 @@
       <c r="F17" s="124" t="s">
         <v>216</v>
       </c>
-      <c r="G17" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H17" s="54">
+      <c r="G17" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H17" s="178">
         <v>45812</v>
       </c>
-      <c r="I17" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K17" s="54">
+      <c r="I17" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K17" s="178">
         <v>45965</v>
       </c>
-      <c r="L17" s="55" t="s">
+      <c r="L17" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M17" s="137"/>
@@ -8270,22 +8305,22 @@
       <c r="F18" s="124" t="s">
         <v>216</v>
       </c>
-      <c r="G18" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H18" s="54">
+      <c r="G18" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H18" s="178">
         <v>45812</v>
       </c>
-      <c r="I18" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K18" s="54">
+      <c r="I18" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K18" s="178">
         <v>45965</v>
       </c>
-      <c r="L18" s="55" t="s">
+      <c r="L18" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M18" s="138"/>
@@ -8309,22 +8344,22 @@
       <c r="F19" s="138" t="s">
         <v>502</v>
       </c>
-      <c r="G19" s="53" t="s">
+      <c r="G19" s="177" t="s">
         <v>489</v>
       </c>
-      <c r="H19" s="54">
+      <c r="H19" s="178">
         <v>45812</v>
       </c>
-      <c r="I19" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K19" s="54">
+      <c r="I19" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K19" s="178">
         <v>45965</v>
       </c>
-      <c r="L19" s="55" t="s">
+      <c r="L19" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M19" s="138"/>
@@ -8348,22 +8383,22 @@
       <c r="F20" s="124" t="s">
         <v>216</v>
       </c>
-      <c r="G20" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="H20" s="54">
+      <c r="G20" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="H20" s="178">
         <v>45812</v>
       </c>
-      <c r="I20" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" s="53" t="s">
-        <v>487</v>
-      </c>
-      <c r="K20" s="54">
+      <c r="I20" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="177" t="s">
+        <v>487</v>
+      </c>
+      <c r="K20" s="178">
         <v>45965</v>
       </c>
-      <c r="L20" s="55" t="s">
+      <c r="L20" s="179" t="s">
         <v>63</v>
       </c>
       <c r="M20" s="138"/>
@@ -8441,13 +8476,6 @@
     <row r="49" ht="103.8" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A10:M10"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -8456,6 +8484,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A10:M10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="J11:J13 J15:J20 G11:G13 G15:G20" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -8473,8 +8508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView topLeftCell="Q18" zoomScale="36" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView zoomScale="51" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -8499,13 +8534,13 @@
       <c r="A1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
       <c r="G1" s="95"/>
       <c r="H1" s="96"/>
       <c r="J1" s="95"/>
@@ -8514,13 +8549,13 @@
       <c r="A2" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="174" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
       <c r="G2" s="95"/>
       <c r="H2" s="96"/>
       <c r="J2" s="95"/>
@@ -8551,10 +8586,10 @@
         <v>46</v>
       </c>
       <c r="B4" s="101">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C4" s="101">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="98">
         <f>COUNTIF(G11:G30,"Untested")</f>
@@ -8564,7 +8599,9 @@
         <f>COUNTIF(G11:G30,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F4" s="98"/>
+      <c r="F4" s="98">
+        <v>34</v>
+      </c>
       <c r="G4" s="95"/>
       <c r="H4" s="96"/>
       <c r="J4" s="95"/>
@@ -8573,7 +8610,9 @@
       <c r="A5" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="101">
+        <v>34</v>
+      </c>
       <c r="C5" s="101">
         <v>0</v>
       </c>
@@ -8585,7 +8624,9 @@
         <f>COUNTIF(J11:J30,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="98"/>
+      <c r="F5" s="98">
+        <v>34</v>
+      </c>
       <c r="G5" s="95"/>
       <c r="H5" s="96"/>
       <c r="J5" s="95"/>
@@ -10046,13 +10087,6 @@
     <row r="69" ht="103.8" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A26:M26"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A10:M10"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -10061,6 +10095,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A10:M10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G11:G25 J11:J25 J27:J45 G27:G45" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -10078,8 +10119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScale="51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -10104,13 +10145,13 @@
       <c r="A1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
       <c r="G1" s="95"/>
       <c r="H1" s="96"/>
       <c r="J1" s="95"/>
@@ -10119,13 +10160,13 @@
       <c r="A2" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="174" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
       <c r="G2" s="95"/>
       <c r="H2" s="96"/>
       <c r="J2" s="95"/>
@@ -10156,10 +10197,10 @@
         <v>46</v>
       </c>
       <c r="B4" s="101">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C4" s="101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="98">
         <f>COUNTIF(G11:G19,"Untested")</f>
@@ -10169,7 +10210,9 @@
         <f>COUNTIF(G11:G19,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F4" s="98"/>
+      <c r="F4" s="98">
+        <v>9</v>
+      </c>
       <c r="G4" s="95"/>
       <c r="H4" s="96"/>
       <c r="J4" s="95"/>
@@ -10178,7 +10221,9 @@
       <c r="A5" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="101">
+        <v>9</v>
+      </c>
       <c r="C5" s="101">
         <v>0</v>
       </c>
@@ -10190,7 +10235,9 @@
         <f>COUNTIF(J11:J19,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="98"/>
+      <c r="F5" s="98">
+        <v>9</v>
+      </c>
       <c r="G5" s="95"/>
       <c r="H5" s="96"/>
       <c r="J5" s="95"/>
@@ -10285,21 +10332,21 @@
       <c r="M9" s="171"/>
     </row>
     <row r="10" spans="1:13" s="97" customFormat="1">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="172" t="s">
         <v>395</v>
       </c>
-      <c r="B10" s="174"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="174"/>
-      <c r="E10" s="174"/>
-      <c r="F10" s="174"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="174"/>
-      <c r="K10" s="174"/>
-      <c r="L10" s="174"/>
-      <c r="M10" s="174"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="172"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="172"/>
+      <c r="L10" s="172"/>
+      <c r="M10" s="172"/>
     </row>
     <row r="11" spans="1:13" s="97" customFormat="1" ht="84">
       <c r="A11" s="108" t="s">
@@ -10553,10 +10600,10 @@
         <v>410</v>
       </c>
       <c r="F18" s="93" t="s">
-        <v>410</v>
+        <v>527</v>
       </c>
       <c r="G18" s="112" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="H18" s="54">
         <v>45812</v>
@@ -10592,10 +10639,10 @@
         <v>366</v>
       </c>
       <c r="F19" s="93" t="s">
-        <v>366</v>
+        <v>528</v>
       </c>
       <c r="G19" s="112" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="H19" s="54">
         <v>45812</v>
@@ -10732,13 +10779,6 @@
     <row r="41" ht="103.8" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A15:M15"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A10:M10"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -10747,6 +10787,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A10:M10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G11:G14 J11:J14 G16:G20 J16:J20" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -10764,8 +10811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="F16" zoomScale="63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView zoomScale="42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -10790,13 +10837,13 @@
       <c r="A1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
       <c r="G1" s="95"/>
       <c r="H1" s="96"/>
       <c r="J1" s="95"/>
@@ -10805,13 +10852,13 @@
       <c r="A2" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="174" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
       <c r="G2" s="95"/>
       <c r="H2" s="96"/>
       <c r="J2" s="95"/>
@@ -10842,10 +10889,10 @@
         <v>46</v>
       </c>
       <c r="B4" s="101">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C4" s="101">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="98">
         <f>COUNTIF(G11:G25,"Untested")</f>
@@ -10855,7 +10902,9 @@
         <f>COUNTIF(G11:G25,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F4" s="98"/>
+      <c r="F4" s="98">
+        <v>18</v>
+      </c>
       <c r="G4" s="95"/>
       <c r="H4" s="96"/>
       <c r="J4" s="95"/>
@@ -10864,7 +10913,9 @@
       <c r="A5" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="101">
+        <v>18</v>
+      </c>
       <c r="C5" s="101">
         <v>0</v>
       </c>
@@ -10876,7 +10927,9 @@
         <f>COUNTIF(J11:J25,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="98"/>
+      <c r="F5" s="98">
+        <v>18</v>
+      </c>
       <c r="G5" s="95"/>
       <c r="H5" s="96"/>
       <c r="J5" s="95"/>
@@ -10971,21 +11024,21 @@
       <c r="M9" s="171"/>
     </row>
     <row r="10" spans="1:13" s="97" customFormat="1">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="172" t="s">
         <v>311</v>
       </c>
-      <c r="B10" s="174"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="174"/>
-      <c r="E10" s="174"/>
-      <c r="F10" s="174"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="174"/>
-      <c r="K10" s="174"/>
-      <c r="L10" s="174"/>
-      <c r="M10" s="174"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="172"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="172"/>
+      <c r="L10" s="172"/>
+      <c r="M10" s="172"/>
     </row>
     <row r="11" spans="1:13" s="97" customFormat="1" ht="84">
       <c r="A11" s="108" t="s">
@@ -11381,12 +11434,18 @@
       <c r="H22" s="54">
         <v>45842</v>
       </c>
-      <c r="I22" s="113"/>
-      <c r="J22" s="112"/>
+      <c r="I22" s="113" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="112" t="s">
+        <v>487</v>
+      </c>
       <c r="K22" s="54">
         <v>45751</v>
       </c>
-      <c r="L22" s="113"/>
+      <c r="L22" s="113" t="s">
+        <v>63</v>
+      </c>
       <c r="M22" s="110"/>
     </row>
     <row r="23" spans="1:13" s="97" customFormat="1" ht="103.8" customHeight="1">
@@ -11737,6 +11796,13 @@
     <row r="50" ht="103.8" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A10:M10"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -11745,16 +11811,9 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A10:M10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G11:G19 J11:J19 J21:J29 G21:G29" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G11:G19 J11:J19 G21:G29 J21:J29" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"Passed,Untested,Failed,Blocked"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>